<commit_message>
hided error on start
</commit_message>
<xml_diff>
--- a/TestExcelWebAddIn1/bin/Debug/Book1.xlsx
+++ b/TestExcelWebAddIn1/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R74a312df92284b63"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rd0ec048ae50a4b3a"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R28b92acf6f3b4d82"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rc939f0eafbd24133"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{349af2c1-5c8b-475f-86a0-b6478d241bb7}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4362e9dc-5881-44f0-9b48-533fc1f70169}">
   <we:reference id="00865d8b-2b8d-4927-b2d9-a6780cf14e28" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
minor fix to position
</commit_message>
<xml_diff>
--- a/TestExcelWebAddIn1/bin/Debug/Book1.xlsx
+++ b/TestExcelWebAddIn1/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rd0ec048ae50a4b3a"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R93932329c0464db5"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rc939f0eafbd24133"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Ra6de0486dd404419"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4362e9dc-5881-44f0-9b48-533fc1f70169}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{37567f01-04dd-4505-a3bd-f467f1e8eb10}">
   <we:reference id="00865d8b-2b8d-4927-b2d9-a6780cf14e28" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>